<commit_message>
*best* Project Results KneighborsClassifier
</commit_message>
<xml_diff>
--- a/project_results.xlsx
+++ b/project_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maren\Python\machineLearningProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842BBAB5-9CB6-4999-94DE-5F03F379C9D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4609DB-63C0-4E86-9323-ECEA0EEB6ACB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11746" activeTab="4" xr2:uid="{DBFDAFC6-5964-47A5-B37B-48FDB3DF0ABC}"/>
   </bookViews>
@@ -115,7 +115,7 @@
     <t>Is_young</t>
   </si>
   <si>
-    <t>KNeighborClassifier</t>
+    <t>KNeighborsClassifier</t>
   </si>
 </sst>
 </file>
@@ -568,13 +568,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -586,10 +583,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1330,196 +1330,196 @@
       <c r="I2" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="120" t="s">
+      <c r="K2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="121"/>
-      <c r="M2" s="117" t="s">
+      <c r="L2" s="115"/>
+      <c r="M2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="118"/>
-      <c r="O2" s="118"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="118"/>
-      <c r="R2" s="118"/>
-      <c r="S2" s="118"/>
-      <c r="T2" s="118"/>
-      <c r="U2" s="118"/>
-      <c r="V2" s="118"/>
-      <c r="W2" s="118"/>
-      <c r="X2" s="118"/>
-      <c r="Y2" s="118"/>
-      <c r="AA2" s="120" t="s">
+      <c r="N2" s="117"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="117"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="117"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="117"/>
+      <c r="Y2" s="117"/>
+      <c r="AA2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="AB2" s="121"/>
-      <c r="AC2" s="117" t="s">
+      <c r="AB2" s="115"/>
+      <c r="AC2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="118"/>
-      <c r="AE2" s="118"/>
-      <c r="AF2" s="118"/>
-      <c r="AG2" s="118"/>
-      <c r="AH2" s="118"/>
-      <c r="AI2" s="118"/>
-      <c r="AJ2" s="118"/>
-      <c r="AK2" s="118"/>
-      <c r="AL2" s="118"/>
-      <c r="AM2" s="118"/>
-      <c r="AN2" s="118"/>
-      <c r="AO2" s="119"/>
-      <c r="AQ2" s="120" t="s">
+      <c r="AD2" s="117"/>
+      <c r="AE2" s="117"/>
+      <c r="AF2" s="117"/>
+      <c r="AG2" s="117"/>
+      <c r="AH2" s="117"/>
+      <c r="AI2" s="117"/>
+      <c r="AJ2" s="117"/>
+      <c r="AK2" s="117"/>
+      <c r="AL2" s="117"/>
+      <c r="AM2" s="117"/>
+      <c r="AN2" s="117"/>
+      <c r="AO2" s="118"/>
+      <c r="AQ2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="AR2" s="121"/>
-      <c r="AS2" s="117" t="s">
+      <c r="AR2" s="115"/>
+      <c r="AS2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="AT2" s="118"/>
-      <c r="AU2" s="118"/>
-      <c r="AV2" s="118"/>
-      <c r="AW2" s="118"/>
-      <c r="AX2" s="118"/>
-      <c r="AY2" s="118"/>
-      <c r="AZ2" s="118"/>
-      <c r="BA2" s="118"/>
-      <c r="BB2" s="118"/>
-      <c r="BC2" s="118"/>
-      <c r="BD2" s="118"/>
-      <c r="BE2" s="119"/>
-      <c r="BG2" s="120" t="s">
+      <c r="AT2" s="117"/>
+      <c r="AU2" s="117"/>
+      <c r="AV2" s="117"/>
+      <c r="AW2" s="117"/>
+      <c r="AX2" s="117"/>
+      <c r="AY2" s="117"/>
+      <c r="AZ2" s="117"/>
+      <c r="BA2" s="117"/>
+      <c r="BB2" s="117"/>
+      <c r="BC2" s="117"/>
+      <c r="BD2" s="117"/>
+      <c r="BE2" s="118"/>
+      <c r="BG2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="BH2" s="121"/>
-      <c r="BI2" s="117" t="s">
+      <c r="BH2" s="115"/>
+      <c r="BI2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="BJ2" s="118"/>
-      <c r="BK2" s="118"/>
-      <c r="BL2" s="118"/>
-      <c r="BM2" s="118"/>
-      <c r="BN2" s="118"/>
-      <c r="BO2" s="118"/>
-      <c r="BP2" s="118"/>
-      <c r="BQ2" s="118"/>
-      <c r="BR2" s="118"/>
-      <c r="BS2" s="118"/>
-      <c r="BT2" s="118"/>
-      <c r="BU2" s="119"/>
-      <c r="BW2" s="120" t="s">
+      <c r="BJ2" s="117"/>
+      <c r="BK2" s="117"/>
+      <c r="BL2" s="117"/>
+      <c r="BM2" s="117"/>
+      <c r="BN2" s="117"/>
+      <c r="BO2" s="117"/>
+      <c r="BP2" s="117"/>
+      <c r="BQ2" s="117"/>
+      <c r="BR2" s="117"/>
+      <c r="BS2" s="117"/>
+      <c r="BT2" s="117"/>
+      <c r="BU2" s="118"/>
+      <c r="BW2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="BX2" s="121"/>
-      <c r="BY2" s="117" t="s">
+      <c r="BX2" s="115"/>
+      <c r="BY2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="BZ2" s="118"/>
-      <c r="CA2" s="118"/>
-      <c r="CB2" s="118"/>
-      <c r="CC2" s="118"/>
-      <c r="CD2" s="118"/>
-      <c r="CE2" s="118"/>
-      <c r="CF2" s="118"/>
-      <c r="CG2" s="118"/>
-      <c r="CH2" s="118"/>
-      <c r="CI2" s="118"/>
-      <c r="CJ2" s="118"/>
-      <c r="CK2" s="119"/>
-      <c r="CM2" s="120" t="s">
+      <c r="BZ2" s="117"/>
+      <c r="CA2" s="117"/>
+      <c r="CB2" s="117"/>
+      <c r="CC2" s="117"/>
+      <c r="CD2" s="117"/>
+      <c r="CE2" s="117"/>
+      <c r="CF2" s="117"/>
+      <c r="CG2" s="117"/>
+      <c r="CH2" s="117"/>
+      <c r="CI2" s="117"/>
+      <c r="CJ2" s="117"/>
+      <c r="CK2" s="118"/>
+      <c r="CM2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="CN2" s="121"/>
-      <c r="CO2" s="117" t="s">
+      <c r="CN2" s="115"/>
+      <c r="CO2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="CP2" s="118"/>
-      <c r="CQ2" s="118"/>
-      <c r="CR2" s="118"/>
-      <c r="CS2" s="118"/>
-      <c r="CT2" s="118"/>
-      <c r="CU2" s="118"/>
-      <c r="CV2" s="118"/>
-      <c r="CW2" s="118"/>
-      <c r="CX2" s="118"/>
-      <c r="CY2" s="118"/>
-      <c r="CZ2" s="118"/>
-      <c r="DA2" s="119"/>
-      <c r="DC2" s="120" t="s">
+      <c r="CP2" s="117"/>
+      <c r="CQ2" s="117"/>
+      <c r="CR2" s="117"/>
+      <c r="CS2" s="117"/>
+      <c r="CT2" s="117"/>
+      <c r="CU2" s="117"/>
+      <c r="CV2" s="117"/>
+      <c r="CW2" s="117"/>
+      <c r="CX2" s="117"/>
+      <c r="CY2" s="117"/>
+      <c r="CZ2" s="117"/>
+      <c r="DA2" s="118"/>
+      <c r="DC2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="DD2" s="121"/>
-      <c r="DE2" s="117" t="s">
+      <c r="DD2" s="115"/>
+      <c r="DE2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="DF2" s="118"/>
-      <c r="DG2" s="118"/>
-      <c r="DH2" s="118"/>
-      <c r="DI2" s="118"/>
-      <c r="DJ2" s="118"/>
-      <c r="DK2" s="118"/>
-      <c r="DL2" s="118"/>
-      <c r="DM2" s="118"/>
-      <c r="DN2" s="118"/>
-      <c r="DO2" s="118"/>
-      <c r="DP2" s="118"/>
-      <c r="DQ2" s="119"/>
-      <c r="DS2" s="120" t="s">
+      <c r="DF2" s="117"/>
+      <c r="DG2" s="117"/>
+      <c r="DH2" s="117"/>
+      <c r="DI2" s="117"/>
+      <c r="DJ2" s="117"/>
+      <c r="DK2" s="117"/>
+      <c r="DL2" s="117"/>
+      <c r="DM2" s="117"/>
+      <c r="DN2" s="117"/>
+      <c r="DO2" s="117"/>
+      <c r="DP2" s="117"/>
+      <c r="DQ2" s="118"/>
+      <c r="DS2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="DT2" s="121"/>
-      <c r="DU2" s="117" t="s">
+      <c r="DT2" s="115"/>
+      <c r="DU2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="DV2" s="118"/>
-      <c r="DW2" s="118"/>
-      <c r="DX2" s="118"/>
-      <c r="DY2" s="118"/>
-      <c r="DZ2" s="118"/>
-      <c r="EA2" s="118"/>
-      <c r="EB2" s="118"/>
-      <c r="EC2" s="118"/>
-      <c r="ED2" s="118"/>
-      <c r="EE2" s="118"/>
-      <c r="EF2" s="118"/>
-      <c r="EG2" s="119"/>
-      <c r="EI2" s="120" t="s">
+      <c r="DV2" s="117"/>
+      <c r="DW2" s="117"/>
+      <c r="DX2" s="117"/>
+      <c r="DY2" s="117"/>
+      <c r="DZ2" s="117"/>
+      <c r="EA2" s="117"/>
+      <c r="EB2" s="117"/>
+      <c r="EC2" s="117"/>
+      <c r="ED2" s="117"/>
+      <c r="EE2" s="117"/>
+      <c r="EF2" s="117"/>
+      <c r="EG2" s="118"/>
+      <c r="EI2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="EJ2" s="121"/>
-      <c r="EK2" s="117" t="s">
+      <c r="EJ2" s="115"/>
+      <c r="EK2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="EL2" s="118"/>
-      <c r="EM2" s="118"/>
-      <c r="EN2" s="118"/>
-      <c r="EO2" s="118"/>
-      <c r="EP2" s="118"/>
-      <c r="EQ2" s="118"/>
-      <c r="ER2" s="118"/>
-      <c r="ES2" s="118"/>
-      <c r="ET2" s="118"/>
-      <c r="EU2" s="118"/>
-      <c r="EV2" s="118"/>
-      <c r="EW2" s="119"/>
-      <c r="EY2" s="120" t="s">
+      <c r="EL2" s="117"/>
+      <c r="EM2" s="117"/>
+      <c r="EN2" s="117"/>
+      <c r="EO2" s="117"/>
+      <c r="EP2" s="117"/>
+      <c r="EQ2" s="117"/>
+      <c r="ER2" s="117"/>
+      <c r="ES2" s="117"/>
+      <c r="ET2" s="117"/>
+      <c r="EU2" s="117"/>
+      <c r="EV2" s="117"/>
+      <c r="EW2" s="118"/>
+      <c r="EY2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="EZ2" s="121"/>
-      <c r="FA2" s="117" t="s">
+      <c r="EZ2" s="115"/>
+      <c r="FA2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="FB2" s="118"/>
-      <c r="FC2" s="118"/>
-      <c r="FD2" s="118"/>
-      <c r="FE2" s="118"/>
-      <c r="FF2" s="118"/>
-      <c r="FG2" s="118"/>
-      <c r="FH2" s="118"/>
-      <c r="FI2" s="118"/>
-      <c r="FJ2" s="118"/>
-      <c r="FK2" s="118"/>
-      <c r="FL2" s="118"/>
-      <c r="FM2" s="119"/>
+      <c r="FB2" s="117"/>
+      <c r="FC2" s="117"/>
+      <c r="FD2" s="117"/>
+      <c r="FE2" s="117"/>
+      <c r="FF2" s="117"/>
+      <c r="FG2" s="117"/>
+      <c r="FH2" s="117"/>
+      <c r="FI2" s="117"/>
+      <c r="FJ2" s="117"/>
+      <c r="FK2" s="117"/>
+      <c r="FL2" s="117"/>
+      <c r="FM2" s="118"/>
       <c r="FO2" s="99"/>
       <c r="FP2" s="99"/>
       <c r="FQ2" s="98"/>
@@ -2107,7 +2107,7 @@
         <v>0.81799999999999995</v>
       </c>
       <c r="Z4" s="33"/>
-      <c r="AA4" s="114" t="s">
+      <c r="AA4" s="119" t="s">
         <v>5</v>
       </c>
       <c r="AB4" s="59" t="s">
@@ -2150,7 +2150,7 @@
       <c r="AO4" s="15">
         <v>0.81899999999999995</v>
       </c>
-      <c r="AQ4" s="114" t="s">
+      <c r="AQ4" s="119" t="s">
         <v>5</v>
       </c>
       <c r="AR4" s="59" t="s">
@@ -2191,7 +2191,7 @@
       <c r="BE4" s="15">
         <v>0.81799999999999995</v>
       </c>
-      <c r="BG4" s="114" t="s">
+      <c r="BG4" s="119" t="s">
         <v>5</v>
       </c>
       <c r="BH4" s="59" t="s">
@@ -2230,7 +2230,7 @@
       <c r="BU4" s="21">
         <v>0.82299999999999995</v>
       </c>
-      <c r="BW4" s="114" t="s">
+      <c r="BW4" s="119" t="s">
         <v>5</v>
       </c>
       <c r="BX4" s="59" t="s">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="CJ4" s="85"/>
       <c r="CK4" s="85"/>
-      <c r="CM4" s="114" t="s">
+      <c r="CM4" s="119" t="s">
         <v>5</v>
       </c>
       <c r="CN4" s="59" t="s">
@@ -2302,7 +2302,7 @@
       </c>
       <c r="CZ4" s="85"/>
       <c r="DA4" s="85"/>
-      <c r="DC4" s="114" t="s">
+      <c r="DC4" s="119" t="s">
         <v>5</v>
       </c>
       <c r="DD4" s="59" t="s">
@@ -2335,7 +2335,7 @@
       </c>
       <c r="DP4" s="85"/>
       <c r="DQ4" s="85"/>
-      <c r="DS4" s="114" t="s">
+      <c r="DS4" s="119" t="s">
         <v>5</v>
       </c>
       <c r="DT4" s="59" t="s">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="EF4" s="85"/>
       <c r="EG4" s="85"/>
-      <c r="EI4" s="114" t="s">
+      <c r="EI4" s="119" t="s">
         <v>5</v>
       </c>
       <c r="EJ4" s="59" t="s">
@@ -2395,7 +2395,7 @@
       </c>
       <c r="EV4" s="85"/>
       <c r="EW4" s="85"/>
-      <c r="EY4" s="114" t="s">
+      <c r="EY4" s="119" t="s">
         <v>5</v>
       </c>
       <c r="EZ4" s="59" t="s">
@@ -2422,7 +2422,7 @@
       </c>
       <c r="FL4" s="85"/>
       <c r="FM4" s="85"/>
-      <c r="FO4" s="114" t="s">
+      <c r="FO4" s="119" t="s">
         <v>5</v>
       </c>
       <c r="FP4" s="59" t="s">
@@ -2510,7 +2510,7 @@
       <c r="Y5" s="22">
         <v>0.81299999999999994</v>
       </c>
-      <c r="AA5" s="115"/>
+      <c r="AA5" s="120"/>
       <c r="AB5" s="63" t="s">
         <v>7</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>0.79800000000000004</v>
       </c>
       <c r="AO5" s="84"/>
-      <c r="AQ5" s="115"/>
+      <c r="AQ5" s="120"/>
       <c r="AR5" s="63" t="s">
         <v>7</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>0.81699999999999995</v>
       </c>
       <c r="BE5" s="84"/>
-      <c r="BG5" s="115"/>
+      <c r="BG5" s="120"/>
       <c r="BH5" s="63" t="s">
         <v>7</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>0.81599999999999995</v>
       </c>
       <c r="BU5" s="84"/>
-      <c r="BW5" s="115"/>
+      <c r="BW5" s="120"/>
       <c r="BX5" s="63" t="s">
         <v>7</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>0.81200000000000006</v>
       </c>
       <c r="CK5" s="84"/>
-      <c r="CM5" s="115"/>
+      <c r="CM5" s="120"/>
       <c r="CN5" s="63" t="s">
         <v>7</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>0.80800000000000005</v>
       </c>
       <c r="DA5" s="84"/>
-      <c r="DC5" s="115"/>
+      <c r="DC5" s="120"/>
       <c r="DD5" s="63" t="s">
         <v>7</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>0.81599999999999995</v>
       </c>
       <c r="DQ5" s="84"/>
-      <c r="DS5" s="115"/>
+      <c r="DS5" s="120"/>
       <c r="DT5" s="63" t="s">
         <v>7</v>
       </c>
@@ -2755,7 +2755,7 @@
       </c>
       <c r="EF5" s="84"/>
       <c r="EG5" s="84"/>
-      <c r="EI5" s="115"/>
+      <c r="EI5" s="120"/>
       <c r="EJ5" s="63" t="s">
         <v>7</v>
       </c>
@@ -2782,7 +2782,7 @@
       </c>
       <c r="EV5" s="84"/>
       <c r="EW5" s="84"/>
-      <c r="EY5" s="115"/>
+      <c r="EY5" s="120"/>
       <c r="EZ5" s="63" t="s">
         <v>7</v>
       </c>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="FL5" s="84"/>
       <c r="FM5" s="84"/>
-      <c r="FO5" s="115"/>
+      <c r="FO5" s="120"/>
       <c r="FP5" s="63" t="s">
         <v>7</v>
       </c>
@@ -2895,7 +2895,7 @@
       <c r="Y6" s="17">
         <v>0.752</v>
       </c>
-      <c r="AA6" s="115"/>
+      <c r="AA6" s="120"/>
       <c r="AB6" s="63" t="s">
         <v>8</v>
       </c>
@@ -2936,7 +2936,7 @@
       <c r="AO6" s="17">
         <v>0.75700000000000001</v>
       </c>
-      <c r="AQ6" s="115"/>
+      <c r="AQ6" s="120"/>
       <c r="AR6" s="63" t="s">
         <v>8</v>
       </c>
@@ -2975,7 +2975,7 @@
       <c r="BE6" s="17">
         <v>0.78900000000000003</v>
       </c>
-      <c r="BG6" s="115"/>
+      <c r="BG6" s="120"/>
       <c r="BH6" s="63" t="s">
         <v>8</v>
       </c>
@@ -3012,7 +3012,7 @@
       <c r="BU6" s="22">
         <v>0.82199999999999995</v>
       </c>
-      <c r="BW6" s="115"/>
+      <c r="BW6" s="120"/>
       <c r="BX6" s="63" t="s">
         <v>8</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>0.79</v>
       </c>
       <c r="CK6" s="84"/>
-      <c r="CM6" s="115"/>
+      <c r="CM6" s="120"/>
       <c r="CN6" s="63" t="s">
         <v>8</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>0.76900000000000002</v>
       </c>
       <c r="DA6" s="84"/>
-      <c r="DC6" s="115"/>
+      <c r="DC6" s="120"/>
       <c r="DD6" s="63" t="s">
         <v>8</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>0.76619999999999999</v>
       </c>
       <c r="DQ6" s="84"/>
-      <c r="DS6" s="115"/>
+      <c r="DS6" s="120"/>
       <c r="DT6" s="63" t="s">
         <v>8</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>0.752</v>
       </c>
       <c r="EG6" s="84"/>
-      <c r="EI6" s="115"/>
+      <c r="EI6" s="120"/>
       <c r="EJ6" s="63" t="s">
         <v>8</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>0.79300000000000004</v>
       </c>
       <c r="EW6" s="84"/>
-      <c r="EY6" s="115"/>
+      <c r="EY6" s="120"/>
       <c r="EZ6" s="63" t="s">
         <v>8</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>0.79300000000000004</v>
       </c>
       <c r="FM6" s="84"/>
-      <c r="FO6" s="115"/>
+      <c r="FO6" s="120"/>
       <c r="FP6" s="63" t="s">
         <v>8</v>
       </c>
@@ -3280,7 +3280,7 @@
       <c r="Y7" s="19">
         <v>0.79300000000000004</v>
       </c>
-      <c r="AA7" s="116"/>
+      <c r="AA7" s="121"/>
       <c r="AB7" s="63" t="s">
         <v>9</v>
       </c>
@@ -3321,7 +3321,7 @@
       <c r="AO7" s="19">
         <v>0.79200000000000004</v>
       </c>
-      <c r="AQ7" s="116"/>
+      <c r="AQ7" s="121"/>
       <c r="AR7" s="63" t="s">
         <v>9</v>
       </c>
@@ -3360,7 +3360,7 @@
       <c r="BE7" s="19">
         <v>0.79700000000000004</v>
       </c>
-      <c r="BG7" s="116"/>
+      <c r="BG7" s="121"/>
       <c r="BH7" s="63" t="s">
         <v>9</v>
       </c>
@@ -3397,7 +3397,7 @@
       <c r="BU7" s="19">
         <v>0.80200000000000005</v>
       </c>
-      <c r="BW7" s="116"/>
+      <c r="BW7" s="121"/>
       <c r="BX7" s="63" t="s">
         <v>9</v>
       </c>
@@ -3432,7 +3432,7 @@
       <c r="CK7" s="19">
         <v>0.8</v>
       </c>
-      <c r="CM7" s="116"/>
+      <c r="CM7" s="121"/>
       <c r="CN7" s="63" t="s">
         <v>9</v>
       </c>
@@ -3465,7 +3465,7 @@
       <c r="DA7" s="19">
         <v>0.81399999999999995</v>
       </c>
-      <c r="DC7" s="116"/>
+      <c r="DC7" s="121"/>
       <c r="DD7" s="63" t="s">
         <v>9</v>
       </c>
@@ -3496,7 +3496,7 @@
       <c r="DQ7" s="24">
         <v>0.80100000000000005</v>
       </c>
-      <c r="DS7" s="116"/>
+      <c r="DS7" s="121"/>
       <c r="DT7" s="63" t="s">
         <v>9</v>
       </c>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="EF7" s="88"/>
       <c r="EG7" s="88"/>
-      <c r="EI7" s="116"/>
+      <c r="EI7" s="121"/>
       <c r="EJ7" s="63" t="s">
         <v>9</v>
       </c>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="EV7" s="88"/>
       <c r="EW7" s="88"/>
-      <c r="EY7" s="116"/>
+      <c r="EY7" s="121"/>
       <c r="EZ7" s="63" t="s">
         <v>9</v>
       </c>
@@ -3577,7 +3577,7 @@
       </c>
       <c r="FL7" s="88"/>
       <c r="FM7" s="88"/>
-      <c r="FO7" s="116"/>
+      <c r="FO7" s="121"/>
       <c r="FP7" s="63" t="s">
         <v>9</v>
       </c>
@@ -7076,24 +7076,31 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="FO8:FO11"/>
-    <mergeCell ref="FO12:FO15"/>
-    <mergeCell ref="EY2:EZ2"/>
-    <mergeCell ref="FA2:FM2"/>
-    <mergeCell ref="FO4:FO7"/>
-    <mergeCell ref="EY12:EY15"/>
-    <mergeCell ref="BW2:BX2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:Y2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AO2"/>
-    <mergeCell ref="AQ2:AR2"/>
-    <mergeCell ref="AS2:BE2"/>
-    <mergeCell ref="BG2:BH2"/>
-    <mergeCell ref="BI2:BU2"/>
+    <mergeCell ref="BW12:BW15"/>
+    <mergeCell ref="CM12:CM15"/>
+    <mergeCell ref="DC12:DC15"/>
+    <mergeCell ref="DS12:DS15"/>
+    <mergeCell ref="EI12:EI15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="AA12:AA15"/>
+    <mergeCell ref="AQ12:AQ15"/>
+    <mergeCell ref="BG12:BG15"/>
+    <mergeCell ref="DC4:DC7"/>
+    <mergeCell ref="DS4:DS7"/>
+    <mergeCell ref="EI4:EI7"/>
+    <mergeCell ref="EY4:EY7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="AA8:AA11"/>
+    <mergeCell ref="AQ8:AQ11"/>
+    <mergeCell ref="BG8:BG11"/>
+    <mergeCell ref="BW8:BW11"/>
+    <mergeCell ref="CM8:CM11"/>
+    <mergeCell ref="DC8:DC11"/>
+    <mergeCell ref="DS8:DS11"/>
+    <mergeCell ref="EI8:EI11"/>
+    <mergeCell ref="EY8:EY11"/>
     <mergeCell ref="DU2:EG2"/>
     <mergeCell ref="EI2:EJ2"/>
     <mergeCell ref="EK2:EW2"/>
@@ -7110,31 +7117,24 @@
     <mergeCell ref="DC2:DD2"/>
     <mergeCell ref="DE2:DQ2"/>
     <mergeCell ref="DS2:DT2"/>
-    <mergeCell ref="DC4:DC7"/>
-    <mergeCell ref="DS4:DS7"/>
-    <mergeCell ref="EI4:EI7"/>
-    <mergeCell ref="EY4:EY7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="AA8:AA11"/>
-    <mergeCell ref="AQ8:AQ11"/>
-    <mergeCell ref="BG8:BG11"/>
-    <mergeCell ref="BW8:BW11"/>
-    <mergeCell ref="CM8:CM11"/>
-    <mergeCell ref="DC8:DC11"/>
-    <mergeCell ref="DS8:DS11"/>
-    <mergeCell ref="EI8:EI11"/>
-    <mergeCell ref="EY8:EY11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="AA12:AA15"/>
-    <mergeCell ref="AQ12:AQ15"/>
-    <mergeCell ref="BG12:BG15"/>
-    <mergeCell ref="BW12:BW15"/>
-    <mergeCell ref="CM12:CM15"/>
-    <mergeCell ref="DC12:DC15"/>
-    <mergeCell ref="DS12:DS15"/>
-    <mergeCell ref="EI12:EI15"/>
+    <mergeCell ref="BW2:BX2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:Y2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AO2"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AS2:BE2"/>
+    <mergeCell ref="BG2:BH2"/>
+    <mergeCell ref="BI2:BU2"/>
+    <mergeCell ref="FO8:FO11"/>
+    <mergeCell ref="FO12:FO15"/>
+    <mergeCell ref="EY2:EZ2"/>
+    <mergeCell ref="FA2:FM2"/>
+    <mergeCell ref="FO4:FO7"/>
+    <mergeCell ref="EY12:EY15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7190,191 +7190,191 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:157" ht="14.55" customHeight="1">
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="120" t="s">
+      <c r="C2" s="115"/>
+      <c r="D2" s="114" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="123"/>
       <c r="F2" s="123"/>
       <c r="G2" s="123"/>
-      <c r="H2" s="121"/>
+      <c r="H2" s="115"/>
       <c r="I2" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="120" t="s">
+      <c r="K2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="121"/>
-      <c r="M2" s="117" t="s">
+      <c r="L2" s="115"/>
+      <c r="M2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="118"/>
-      <c r="O2" s="118"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="118"/>
-      <c r="R2" s="118"/>
-      <c r="S2" s="118"/>
-      <c r="T2" s="118"/>
-      <c r="U2" s="118"/>
-      <c r="V2" s="118"/>
-      <c r="W2" s="118"/>
-      <c r="X2" s="118"/>
-      <c r="Y2" s="118"/>
-      <c r="AA2" s="120" t="s">
+      <c r="N2" s="117"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="117"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="117"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="117"/>
+      <c r="Y2" s="117"/>
+      <c r="AA2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="AB2" s="121"/>
-      <c r="AC2" s="117" t="s">
+      <c r="AB2" s="115"/>
+      <c r="AC2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="118"/>
-      <c r="AE2" s="118"/>
-      <c r="AF2" s="118"/>
-      <c r="AG2" s="118"/>
-      <c r="AH2" s="118"/>
-      <c r="AI2" s="118"/>
-      <c r="AJ2" s="118"/>
-      <c r="AK2" s="118"/>
-      <c r="AL2" s="118"/>
-      <c r="AM2" s="118"/>
-      <c r="AN2" s="118"/>
-      <c r="AO2" s="119"/>
-      <c r="AQ2" s="120" t="s">
+      <c r="AD2" s="117"/>
+      <c r="AE2" s="117"/>
+      <c r="AF2" s="117"/>
+      <c r="AG2" s="117"/>
+      <c r="AH2" s="117"/>
+      <c r="AI2" s="117"/>
+      <c r="AJ2" s="117"/>
+      <c r="AK2" s="117"/>
+      <c r="AL2" s="117"/>
+      <c r="AM2" s="117"/>
+      <c r="AN2" s="117"/>
+      <c r="AO2" s="118"/>
+      <c r="AQ2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="AR2" s="121"/>
-      <c r="AS2" s="117" t="s">
+      <c r="AR2" s="115"/>
+      <c r="AS2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="AT2" s="118"/>
-      <c r="AU2" s="118"/>
-      <c r="AV2" s="118"/>
-      <c r="AW2" s="118"/>
-      <c r="AX2" s="118"/>
-      <c r="AY2" s="118"/>
-      <c r="AZ2" s="118"/>
-      <c r="BA2" s="118"/>
-      <c r="BB2" s="118"/>
-      <c r="BC2" s="118"/>
-      <c r="BD2" s="118"/>
-      <c r="BE2" s="119"/>
-      <c r="BG2" s="120" t="s">
+      <c r="AT2" s="117"/>
+      <c r="AU2" s="117"/>
+      <c r="AV2" s="117"/>
+      <c r="AW2" s="117"/>
+      <c r="AX2" s="117"/>
+      <c r="AY2" s="117"/>
+      <c r="AZ2" s="117"/>
+      <c r="BA2" s="117"/>
+      <c r="BB2" s="117"/>
+      <c r="BC2" s="117"/>
+      <c r="BD2" s="117"/>
+      <c r="BE2" s="118"/>
+      <c r="BG2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="BH2" s="121"/>
-      <c r="BI2" s="117" t="s">
+      <c r="BH2" s="115"/>
+      <c r="BI2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="BJ2" s="118"/>
-      <c r="BK2" s="118"/>
-      <c r="BL2" s="118"/>
-      <c r="BM2" s="118"/>
-      <c r="BN2" s="118"/>
-      <c r="BO2" s="118"/>
-      <c r="BP2" s="118"/>
-      <c r="BQ2" s="118"/>
-      <c r="BR2" s="118"/>
-      <c r="BS2" s="118"/>
-      <c r="BT2" s="118"/>
-      <c r="BU2" s="119"/>
-      <c r="BW2" s="120" t="s">
+      <c r="BJ2" s="117"/>
+      <c r="BK2" s="117"/>
+      <c r="BL2" s="117"/>
+      <c r="BM2" s="117"/>
+      <c r="BN2" s="117"/>
+      <c r="BO2" s="117"/>
+      <c r="BP2" s="117"/>
+      <c r="BQ2" s="117"/>
+      <c r="BR2" s="117"/>
+      <c r="BS2" s="117"/>
+      <c r="BT2" s="117"/>
+      <c r="BU2" s="118"/>
+      <c r="BW2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="BX2" s="121"/>
-      <c r="BY2" s="117" t="s">
+      <c r="BX2" s="115"/>
+      <c r="BY2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="BZ2" s="118"/>
-      <c r="CA2" s="118"/>
-      <c r="CB2" s="118"/>
-      <c r="CC2" s="118"/>
-      <c r="CD2" s="118"/>
-      <c r="CE2" s="118"/>
-      <c r="CF2" s="118"/>
-      <c r="CG2" s="118"/>
-      <c r="CH2" s="118"/>
-      <c r="CI2" s="118"/>
-      <c r="CJ2" s="118"/>
-      <c r="CK2" s="119"/>
-      <c r="CM2" s="120" t="s">
+      <c r="BZ2" s="117"/>
+      <c r="CA2" s="117"/>
+      <c r="CB2" s="117"/>
+      <c r="CC2" s="117"/>
+      <c r="CD2" s="117"/>
+      <c r="CE2" s="117"/>
+      <c r="CF2" s="117"/>
+      <c r="CG2" s="117"/>
+      <c r="CH2" s="117"/>
+      <c r="CI2" s="117"/>
+      <c r="CJ2" s="117"/>
+      <c r="CK2" s="118"/>
+      <c r="CM2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="CN2" s="121"/>
-      <c r="CO2" s="117" t="s">
+      <c r="CN2" s="115"/>
+      <c r="CO2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="CP2" s="118"/>
-      <c r="CQ2" s="118"/>
-      <c r="CR2" s="118"/>
-      <c r="CS2" s="118"/>
-      <c r="CT2" s="118"/>
-      <c r="CU2" s="118"/>
-      <c r="CV2" s="118"/>
-      <c r="CW2" s="118"/>
-      <c r="CX2" s="118"/>
-      <c r="CY2" s="118"/>
-      <c r="CZ2" s="118"/>
-      <c r="DA2" s="119"/>
-      <c r="DC2" s="120" t="s">
+      <c r="CP2" s="117"/>
+      <c r="CQ2" s="117"/>
+      <c r="CR2" s="117"/>
+      <c r="CS2" s="117"/>
+      <c r="CT2" s="117"/>
+      <c r="CU2" s="117"/>
+      <c r="CV2" s="117"/>
+      <c r="CW2" s="117"/>
+      <c r="CX2" s="117"/>
+      <c r="CY2" s="117"/>
+      <c r="CZ2" s="117"/>
+      <c r="DA2" s="118"/>
+      <c r="DC2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="DD2" s="121"/>
-      <c r="DE2" s="117" t="s">
+      <c r="DD2" s="115"/>
+      <c r="DE2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="DF2" s="118"/>
-      <c r="DG2" s="118"/>
-      <c r="DH2" s="118"/>
-      <c r="DI2" s="118"/>
-      <c r="DJ2" s="118"/>
-      <c r="DK2" s="118"/>
-      <c r="DL2" s="118"/>
-      <c r="DM2" s="118"/>
-      <c r="DN2" s="118"/>
-      <c r="DO2" s="118"/>
-      <c r="DP2" s="118"/>
-      <c r="DQ2" s="119"/>
-      <c r="DS2" s="120" t="s">
+      <c r="DF2" s="117"/>
+      <c r="DG2" s="117"/>
+      <c r="DH2" s="117"/>
+      <c r="DI2" s="117"/>
+      <c r="DJ2" s="117"/>
+      <c r="DK2" s="117"/>
+      <c r="DL2" s="117"/>
+      <c r="DM2" s="117"/>
+      <c r="DN2" s="117"/>
+      <c r="DO2" s="117"/>
+      <c r="DP2" s="117"/>
+      <c r="DQ2" s="118"/>
+      <c r="DS2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="DT2" s="121"/>
-      <c r="DU2" s="117" t="s">
+      <c r="DT2" s="115"/>
+      <c r="DU2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="DV2" s="118"/>
-      <c r="DW2" s="118"/>
-      <c r="DX2" s="118"/>
-      <c r="DY2" s="118"/>
-      <c r="DZ2" s="118"/>
-      <c r="EA2" s="118"/>
-      <c r="EB2" s="118"/>
-      <c r="EC2" s="118"/>
-      <c r="ED2" s="118"/>
-      <c r="EE2" s="118"/>
-      <c r="EF2" s="118"/>
-      <c r="EG2" s="119"/>
-      <c r="EI2" s="120" t="s">
+      <c r="DV2" s="117"/>
+      <c r="DW2" s="117"/>
+      <c r="DX2" s="117"/>
+      <c r="DY2" s="117"/>
+      <c r="DZ2" s="117"/>
+      <c r="EA2" s="117"/>
+      <c r="EB2" s="117"/>
+      <c r="EC2" s="117"/>
+      <c r="ED2" s="117"/>
+      <c r="EE2" s="117"/>
+      <c r="EF2" s="117"/>
+      <c r="EG2" s="118"/>
+      <c r="EI2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="EJ2" s="121"/>
-      <c r="EK2" s="117" t="s">
+      <c r="EJ2" s="115"/>
+      <c r="EK2" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="EL2" s="118"/>
-      <c r="EM2" s="118"/>
-      <c r="EN2" s="118"/>
-      <c r="EO2" s="118"/>
-      <c r="EP2" s="118"/>
-      <c r="EQ2" s="118"/>
-      <c r="ER2" s="118"/>
-      <c r="ES2" s="118"/>
-      <c r="ET2" s="118"/>
-      <c r="EU2" s="118"/>
-      <c r="EV2" s="118"/>
-      <c r="EW2" s="119"/>
+      <c r="EL2" s="117"/>
+      <c r="EM2" s="117"/>
+      <c r="EN2" s="117"/>
+      <c r="EO2" s="117"/>
+      <c r="EP2" s="117"/>
+      <c r="EQ2" s="117"/>
+      <c r="ER2" s="117"/>
+      <c r="ES2" s="117"/>
+      <c r="ET2" s="117"/>
+      <c r="EU2" s="117"/>
+      <c r="EV2" s="117"/>
+      <c r="EW2" s="118"/>
     </row>
     <row r="3" spans="2:157">
       <c r="B3" s="66" t="s">
@@ -8113,7 +8113,7 @@
       <c r="EU4" s="51"/>
       <c r="EV4" s="48"/>
       <c r="EW4" s="48"/>
-      <c r="EY4" s="114" t="s">
+      <c r="EY4" s="119" t="s">
         <v>5</v>
       </c>
       <c r="EZ4" s="59" t="s">
@@ -8429,7 +8429,7 @@
       <c r="EU5" s="43"/>
       <c r="EV5" s="43"/>
       <c r="EW5" s="43"/>
-      <c r="EY5" s="115"/>
+      <c r="EY5" s="120"/>
       <c r="EZ5" s="63" t="s">
         <v>7</v>
       </c>
@@ -8693,7 +8693,7 @@
       <c r="EU6" s="43"/>
       <c r="EV6" s="43"/>
       <c r="EW6" s="43"/>
-      <c r="EY6" s="115"/>
+      <c r="EY6" s="120"/>
       <c r="EZ6" s="63" t="s">
         <v>8</v>
       </c>
@@ -8995,7 +8995,7 @@
       <c r="EU7" s="58"/>
       <c r="EV7" s="56"/>
       <c r="EW7" s="56"/>
-      <c r="EY7" s="116"/>
+      <c r="EY7" s="121"/>
       <c r="EZ7" s="63" t="s">
         <v>9</v>
       </c>
@@ -12135,19 +12135,32 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="EK2:EW2"/>
-    <mergeCell ref="EI4:EI7"/>
-    <mergeCell ref="EI8:EI11"/>
-    <mergeCell ref="EI12:EI15"/>
-    <mergeCell ref="EY4:EY7"/>
-    <mergeCell ref="EY8:EY11"/>
-    <mergeCell ref="EY12:EY15"/>
-    <mergeCell ref="EI2:EJ2"/>
-    <mergeCell ref="DS2:DT2"/>
-    <mergeCell ref="DU2:EG2"/>
-    <mergeCell ref="DS4:DS7"/>
-    <mergeCell ref="DS8:DS11"/>
-    <mergeCell ref="DS12:DS15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:Y2"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="BI2:BU2"/>
+    <mergeCell ref="BG4:BG7"/>
+    <mergeCell ref="BG8:BG11"/>
+    <mergeCell ref="BG12:BG15"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AO2"/>
+    <mergeCell ref="AA4:AA7"/>
+    <mergeCell ref="AA8:AA11"/>
+    <mergeCell ref="AA12:AA15"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AS2:BE2"/>
+    <mergeCell ref="AQ4:AQ7"/>
+    <mergeCell ref="AQ8:AQ11"/>
+    <mergeCell ref="AQ12:AQ15"/>
+    <mergeCell ref="BG2:BH2"/>
     <mergeCell ref="DE2:DQ2"/>
     <mergeCell ref="DC4:DC7"/>
     <mergeCell ref="DC8:DC11"/>
@@ -12163,32 +12176,19 @@
     <mergeCell ref="CM8:CM11"/>
     <mergeCell ref="CM12:CM15"/>
     <mergeCell ref="DC2:DD2"/>
-    <mergeCell ref="BI2:BU2"/>
-    <mergeCell ref="BG4:BG7"/>
-    <mergeCell ref="BG8:BG11"/>
-    <mergeCell ref="BG12:BG15"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AO2"/>
-    <mergeCell ref="AA4:AA7"/>
-    <mergeCell ref="AA8:AA11"/>
-    <mergeCell ref="AA12:AA15"/>
-    <mergeCell ref="AQ2:AR2"/>
-    <mergeCell ref="AS2:BE2"/>
-    <mergeCell ref="AQ4:AQ7"/>
-    <mergeCell ref="AQ8:AQ11"/>
-    <mergeCell ref="AQ12:AQ15"/>
-    <mergeCell ref="BG2:BH2"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:Y2"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="DS2:DT2"/>
+    <mergeCell ref="DU2:EG2"/>
+    <mergeCell ref="DS4:DS7"/>
+    <mergeCell ref="DS8:DS11"/>
+    <mergeCell ref="DS12:DS15"/>
+    <mergeCell ref="EK2:EW2"/>
+    <mergeCell ref="EI4:EI7"/>
+    <mergeCell ref="EI8:EI11"/>
+    <mergeCell ref="EI12:EI15"/>
+    <mergeCell ref="EY4:EY7"/>
+    <mergeCell ref="EY8:EY11"/>
+    <mergeCell ref="EY12:EY15"/>
+    <mergeCell ref="EI2:EJ2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -12557,7 +12557,7 @@
   <dimension ref="B3:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -12898,12 +12898,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B13:B16"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:H3"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B13:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>